<commit_message>
still trying to make lfs work
</commit_message>
<xml_diff>
--- a/EXPERIMENTATIONS.xlsx
+++ b/EXPERIMENTATIONS.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="results" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="59">
   <si>
     <t>N</t>
   </si>
@@ -116,12 +116,90 @@
   <si>
     <t>4831, 14474</t>
   </si>
+  <si>
+    <t>2000px/class on both</t>
+  </si>
+  <si>
+    <t>1000px/class on both</t>
+  </si>
+  <si>
+    <t>500 px/class on both</t>
+  </si>
+  <si>
+    <t>250 px/class on both</t>
+  </si>
+  <si>
+    <t>100 px/class on both</t>
+  </si>
+  <si>
+    <t>2000px/class for im1, 1000 for im2</t>
+  </si>
+  <si>
+    <t>2000px/class im1, 100 im2</t>
+  </si>
+  <si>
+    <t>2000px/class for im1, 250 for im2</t>
+  </si>
+  <si>
+    <t>2000px/class for im1, 500 for im2</t>
+  </si>
+  <si>
+    <t>1000px/class im1, 500 im2</t>
+  </si>
+  <si>
+    <t>1000px/class im1, 250 im2</t>
+  </si>
+  <si>
+    <t>1000px/class im1,100 im2</t>
+  </si>
+  <si>
+    <t>500px/class im1, 250 im2</t>
+  </si>
+  <si>
+    <t>500px/class im1, 100 im2</t>
+  </si>
+  <si>
+    <t>250px/class im1, 100 im2</t>
+  </si>
+  <si>
+    <t>cf. conf. matrixes sheet</t>
+  </si>
+  <si>
+    <t>exp_89_2000.mat</t>
+  </si>
+  <si>
+    <t>exp_66_2000.mat</t>
+  </si>
+  <si>
+    <t>exp_89_1000.mat</t>
+  </si>
+  <si>
+    <t>exp_66_1000.mat</t>
+  </si>
+  <si>
+    <t>exp_89_500.mat</t>
+  </si>
+  <si>
+    <t>exp_66_500.mat</t>
+  </si>
+  <si>
+    <t>exp_89_250.mat</t>
+  </si>
+  <si>
+    <t>exp_66_250.mat</t>
+  </si>
+  <si>
+    <t>exp_89_100.mat</t>
+  </si>
+  <si>
+    <t>exp_66_100.mat</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -129,13 +207,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.34998626667073579"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="27">
@@ -438,7 +529,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -471,6 +562,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -772,22 +864,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q31"/>
+  <dimension ref="A1:Q256"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.85546875" customWidth="1"/>
     <col min="2" max="2" width="32.5703125" customWidth="1"/>
-    <col min="3" max="3" width="11" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" customWidth="1"/>
     <col min="4" max="4" width="21.42578125" customWidth="1"/>
     <col min="5" max="5" width="19.28515625" customWidth="1"/>
     <col min="6" max="6" width="9.140625" style="4"/>
     <col min="7" max="7" width="22.42578125" style="5" customWidth="1"/>
-    <col min="8" max="8" width="19.7109375" style="5" customWidth="1"/>
+    <col min="8" max="8" width="22" style="5" customWidth="1"/>
     <col min="9" max="9" width="9.140625" style="5"/>
     <col min="10" max="10" width="12.7109375" style="5" customWidth="1"/>
     <col min="11" max="11" width="13.7109375" style="5" customWidth="1"/>
@@ -977,6 +1069,12 @@
       <c r="F4" s="4">
         <v>92.020700000000005</v>
       </c>
+      <c r="G4" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="H4" s="32" t="s">
+        <v>48</v>
+      </c>
       <c r="I4" s="5">
         <v>0.80249999999999999</v>
       </c>
@@ -1024,6 +1122,12 @@
       <c r="F5" s="4">
         <v>89.288300000000007</v>
       </c>
+      <c r="G5" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="H5" s="32" t="s">
+        <v>48</v>
+      </c>
       <c r="I5" s="9">
         <v>0.74860000000000004</v>
       </c>
@@ -1056,226 +1160,526 @@
       <c r="A6" s="15">
         <v>5</v>
       </c>
-      <c r="B6" s="5"/>
+      <c r="B6" s="9" t="s">
+        <v>33</v>
+      </c>
       <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
+      <c r="D6" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="G6" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="H6" s="32" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="15">
         <v>6</v>
       </c>
-      <c r="B7" s="5"/>
+      <c r="B7" s="9" t="s">
+        <v>34</v>
+      </c>
       <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
+      <c r="D7" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="G7" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="H7" s="32" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="15">
         <v>7</v>
       </c>
-      <c r="B8" s="5"/>
+      <c r="B8" s="9" t="s">
+        <v>35</v>
+      </c>
       <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
+      <c r="D8" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="G8" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="H8" s="32" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="15">
         <v>8</v>
       </c>
-      <c r="B9" s="5"/>
+      <c r="B9" s="9" t="s">
+        <v>36</v>
+      </c>
       <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
+      <c r="D9" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="G9" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="H9" s="32" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="15">
         <v>9</v>
       </c>
-      <c r="B10" s="5"/>
+      <c r="B10" s="9" t="s">
+        <v>37</v>
+      </c>
       <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
+      <c r="D10" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="G10" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="H10" s="32" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="15">
         <v>10</v>
       </c>
-      <c r="B11" s="5"/>
+      <c r="B11" s="9" t="s">
+        <v>38</v>
+      </c>
       <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
+      <c r="D11" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="G11" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="H11" s="32" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="15">
         <v>11</v>
       </c>
-      <c r="B12" s="5"/>
+      <c r="B12" s="9" t="s">
+        <v>41</v>
+      </c>
       <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
+      <c r="D12" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="G12" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="H12" s="32" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="15">
         <v>12</v>
       </c>
-      <c r="B13" s="5"/>
+      <c r="B13" s="9" t="s">
+        <v>40</v>
+      </c>
       <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
+      <c r="D13" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="G13" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="H13" s="32" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="15">
         <v>13</v>
       </c>
-      <c r="B14" s="5"/>
+      <c r="B14" s="9" t="s">
+        <v>39</v>
+      </c>
       <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
+      <c r="D14" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="G14" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="H14" s="32" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="15">
         <v>14</v>
       </c>
-      <c r="B15" s="5"/>
+      <c r="B15" s="9" t="s">
+        <v>42</v>
+      </c>
       <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
+      <c r="D15" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="G15" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="H15" s="32" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="15">
         <v>15</v>
       </c>
-      <c r="B16" s="5"/>
+      <c r="B16" s="9" t="s">
+        <v>43</v>
+      </c>
       <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
+      <c r="D16" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="G16" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="H16" s="32" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="15">
         <v>16</v>
       </c>
-      <c r="B17" s="5"/>
+      <c r="B17" s="9" t="s">
+        <v>44</v>
+      </c>
       <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
+      <c r="D17" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="G17" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="H17" s="32" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="15">
         <v>17</v>
       </c>
-      <c r="B18" s="5"/>
+      <c r="B18" s="9" t="s">
+        <v>45</v>
+      </c>
       <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
+      <c r="D18" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="G18" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="H18" s="32" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="15">
         <v>18</v>
       </c>
-      <c r="B19" s="5"/>
+      <c r="B19" s="9" t="s">
+        <v>46</v>
+      </c>
       <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
+      <c r="D19" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="G19" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="H19" s="32" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="15">
         <v>19</v>
       </c>
-      <c r="B20" s="5"/>
+      <c r="B20" s="9" t="s">
+        <v>47</v>
+      </c>
       <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
+      <c r="D20" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="G20" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="H20" s="32" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="15">
         <v>20</v>
       </c>
-      <c r="B21" s="5"/>
+      <c r="B21" s="9" t="s">
+        <v>38</v>
+      </c>
       <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
+      <c r="D21" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="G21" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="H21" s="32" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="15">
         <v>21</v>
       </c>
-      <c r="B22" s="5"/>
+      <c r="B22" s="9" t="s">
+        <v>41</v>
+      </c>
       <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
+      <c r="D22" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="G22" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="H22" s="32" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="15">
         <v>22</v>
       </c>
-      <c r="B23" s="5"/>
+      <c r="B23" s="9" t="s">
+        <v>40</v>
+      </c>
       <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
+      <c r="D23" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="G23" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="H23" s="32" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="15">
         <v>23</v>
       </c>
-      <c r="B24" s="5"/>
+      <c r="B24" s="9" t="s">
+        <v>39</v>
+      </c>
       <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
+      <c r="D24" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="G24" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="H24" s="32" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="15">
         <v>24</v>
       </c>
-      <c r="B25" s="5"/>
+      <c r="B25" s="9" t="s">
+        <v>42</v>
+      </c>
       <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
+      <c r="D25" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="G25" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="H25" s="32" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="15">
         <v>25</v>
       </c>
-      <c r="B26" s="5"/>
+      <c r="B26" s="9" t="s">
+        <v>43</v>
+      </c>
       <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
+      <c r="D26" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="G26" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="H26" s="32" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="15">
         <v>26</v>
       </c>
-      <c r="B27" s="5"/>
+      <c r="B27" s="9" t="s">
+        <v>44</v>
+      </c>
       <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
+      <c r="D27" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="G27" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="H27" s="32" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="15">
         <v>27</v>
       </c>
-      <c r="B28" s="5"/>
+      <c r="B28" s="9" t="s">
+        <v>45</v>
+      </c>
       <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
+      <c r="D28" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="G28" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="H28" s="32" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="15">
         <v>28</v>
       </c>
-      <c r="B29" s="5"/>
+      <c r="B29" s="9" t="s">
+        <v>46</v>
+      </c>
       <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
+      <c r="D29" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E29" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="G29" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="H29" s="32" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="15">
         <v>29</v>
       </c>
-      <c r="B30" s="5"/>
+      <c r="B30" s="9" t="s">
+        <v>47</v>
+      </c>
       <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
+      <c r="D30" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E30" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="G30" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="H30" s="32" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="31" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="16">
@@ -1286,14 +1690,1144 @@
       <c r="D31" s="8"/>
       <c r="E31" s="8"/>
       <c r="F31" s="7"/>
-      <c r="G31" s="8"/>
-      <c r="H31" s="8"/>
+      <c r="G31" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="H31" s="32" t="s">
+        <v>48</v>
+      </c>
       <c r="I31" s="8"/>
       <c r="J31" s="8"/>
       <c r="N31" s="8"/>
     </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A32" s="15">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="15">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="15">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="15">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="15">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="15">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="15">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="15">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="15">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="15">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="15">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="15">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="15">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" s="15">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" s="15">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" s="15">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" s="15">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="15">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="15">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="15">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="15">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="15">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="15">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" s="15">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" s="15">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" s="15">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" s="15">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" s="15">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="16">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" s="15">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" s="15">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" s="15">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="15">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="15">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" s="15">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="15">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" s="15">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" s="15">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" s="15">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" s="15">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" s="15">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" s="15">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" s="15">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" s="15">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" s="15">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" s="15">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" s="15">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" s="15">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" s="15">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" s="15">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" s="15">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" s="15">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" s="15">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" s="15">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" s="15">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" s="15">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" s="15">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" s="15">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A91" s="16">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" s="15">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" s="15">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" s="15">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" s="15">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" s="15">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" s="15">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" s="15">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" s="15">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" s="15">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" s="15">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" s="15">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103" s="15">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104" s="15">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105" s="15">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106" s="15">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A107" s="15">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108" s="15">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A109" s="15">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A110" s="15">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A111" s="15">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A112" s="15">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A113" s="15">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A114" s="15">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A115" s="15">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A116" s="15">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A117" s="15">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A118" s="15">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A119" s="15">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A120" s="15">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A121" s="16">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A122" s="15">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A123" s="15">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A124" s="15">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A125" s="15">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A126" s="15">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A127" s="15">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A128" s="15">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A129" s="15">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A130" s="15">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A131" s="15">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A132" s="15">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A133" s="15">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A134" s="15">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A135" s="15">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A136" s="15">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A137" s="15">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A138" s="15">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A139" s="15">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A140" s="15">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A141" s="15">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A142" s="15">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A143" s="15">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A144" s="15">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A145" s="15">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A146" s="15">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A147" s="15">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A148" s="15">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A149" s="15">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A150" s="15">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A151" s="16">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A152" s="15">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A153" s="15">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A154" s="15">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A155" s="15">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A156" s="15">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A157" s="15">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A158" s="15">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A159" s="15">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A160" s="15">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A161" s="15">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A162" s="15">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A163" s="15">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A164" s="15">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A165" s="15">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A166" s="15">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A167" s="15">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A168" s="15">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A169" s="15">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A170" s="15">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A171" s="15">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A172" s="15">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A173" s="15">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A174" s="15">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A175" s="15">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A176" s="15">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A177" s="15">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A178" s="15">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A179" s="15">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A180" s="15">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A181" s="16">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A182" s="15">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A183" s="15">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A184" s="15">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A185" s="15">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A186" s="15">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A187" s="15">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A188" s="15">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A189" s="15">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A190" s="15">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A191" s="15">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A192" s="15">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A193" s="15">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A194" s="15">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A195" s="15">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A196" s="15">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A197" s="15">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A198" s="15">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A199" s="15">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A200" s="15">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A201" s="15">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A202" s="15">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A203" s="15">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A204" s="15">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A205" s="15">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A206" s="15">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="207" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A207" s="15">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="208" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A208" s="15">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="209" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A209" s="15">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="210" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A210" s="15">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="211" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A211" s="16">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="212" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A212" s="15">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="213" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A213" s="15">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="214" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A214" s="15">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="215" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A215" s="15">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="216" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A216" s="15">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="217" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A217" s="15">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="218" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A218" s="15">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="219" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A219" s="15">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="220" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A220" s="15">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="221" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A221" s="15">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="222" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A222" s="15">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="223" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A223" s="15">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="224" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A224" s="15">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="225" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A225" s="15">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="226" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A226" s="15">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="227" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A227" s="15">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="228" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A228" s="15">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="229" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A229" s="15">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="230" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A230" s="15">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="231" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A231" s="15">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="232" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A232" s="15">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="233" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A233" s="15">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="234" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A234" s="15">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="235" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A235" s="15">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="236" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A236" s="15">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="237" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A237" s="15">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="238" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A238" s="15">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="239" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A239" s="15">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="240" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A240" s="15">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="241" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A241" s="16">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="242" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A242" s="15">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="243" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A243" s="15">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="244" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A244" s="15">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="245" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A245" s="15">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="246" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A246" s="15">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="247" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A247" s="15">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="248" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A248" s="15">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="249" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A249" s="15">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="250" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A250" s="15">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="251" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A251" s="15">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="252" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A252" s="15">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="253" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A253" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="254" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A254" s="15">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="255" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A255" s="15">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="256" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A256" s="15">
+        <v>255</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1301,7 +2835,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K309"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>

</xml_diff>